<commit_message>
Add product html scrap
</commit_message>
<xml_diff>
--- a/fanhouse.xlsx
+++ b/fanhouse.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="59">
   <si>
     <t>No.</t>
   </si>
@@ -31,7 +31,22 @@
     <t>Image</t>
   </si>
   <si>
-    <t>Image2</t>
+    <t>【PRE-SALE】《洋花在置物櫃裡幹嘛?!》 Acrylic Stand　／SLAM DUNK　YouHana　Goods　BY：miau</t>
+  </si>
+  <si>
+    <t>https://fanhouse.waca.ec/en/product/detail/1779106</t>
+  </si>
+  <si>
+    <t>$290</t>
+  </si>
+  <si>
+    <t>【PRE-SALE】《暗潮》　／SLAM DUNK　YouHana　Comic　BY：miau</t>
+  </si>
+  <si>
+    <t>https://fanhouse.waca.ec/en/product/detail/1779088</t>
+  </si>
+  <si>
+    <t>$230</t>
   </si>
   <si>
     <t>《喜歡大快朵頤的你》　／SLAM DUNK　RuHana　Comic　BY：妹子（OiMO）</t>
@@ -40,12 +55,6 @@
     <t>https://fanhouse.waca.ec/en/product/detail/1775678</t>
   </si>
   <si>
-    <t>$230</t>
-  </si>
-  <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/6f/6fb83165c565e5c48269915702968b58.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】《仙道今天渣了嗎？》　／SLAM DUNK　Senru　Novel　BY：HonmeiChoko</t>
   </si>
   <si>
@@ -55,9 +64,6 @@
     <t>$340</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/f9/f9683146ece7dd269bfea62f9314e914.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】Joongdok's Aquarium Date Acrylic Charms 　／Omniscient Reader's Viewpoint　Joongdok　Goods　BY：Hulu呼嚕（剪紙舍）</t>
   </si>
   <si>
@@ -67,9 +73,6 @@
     <t>$120</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/d5/d5d4e6d9ad80ccc7210048e9230474f2.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】Year of the Dragon PP Box　／Omniscient Reader's Viewpoint　Goods　BY：Hulu呼嚕（剪紙舍）</t>
   </si>
   <si>
@@ -79,9 +82,6 @@
     <t>$210</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/2b/2b238394cd780ff1c27b43d221210b94.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】《願能在你的身旁安睡》　／SLAM DUNK　Sawakita Eiji/Rukawa Kaede　Novel　BY：壹依</t>
   </si>
   <si>
@@ -91,9 +91,6 @@
     <t>$300</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/8e/8e307e5a772e9fe6d878a8998376fd6d.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】《無懼》　／SLAM DUNK　RuHana　Novel　BY：穩玟</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>$330</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/c0/c00bc0fc4cd46c5fa96280976b4724aa.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】《我的老公是外星人》　／SLAM DUNK　Sawakita/Fukatsu　Novel　BY：穩玟</t>
   </si>
   <si>
@@ -115,18 +109,12 @@
     <t>$280</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/fa/fae8ecd0ab5eaf3fb0663f52c4ddc581.jpg</t>
-  </si>
-  <si>
     <t>《You Are The One》　／SLAM DUNK　YouHana　Novel　BY：紫筠</t>
   </si>
   <si>
     <t>https://fanhouse.waca.ec/en/product/detail/1775447</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/de/def32dcb6932cb2a8f0ee0dae1a91180.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】《致我親愛的 It's ALL -for you-》　／IDOLiSH7　Yuki/Momo　Novel　BY：夜蒑（Butterfly Effect）</t>
   </si>
   <si>
@@ -136,9 +124,6 @@
     <t>$400</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/9a/9aee0539060d12ac654e04a62f64e04f.jpg</t>
-  </si>
-  <si>
     <t>Goosmav／Roosmav 3cm Acrylic Blocks　／Top Gun:Maverick　Goosmav／Roosmav　Goods　BY：波小姐(LADY PO)（泡在大槍裡的吸貓太太）</t>
   </si>
   <si>
@@ -148,9 +133,6 @@
     <t>$90</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/4a/4afdbaffd8a2934af06a3c211b94fca7.jpg</t>
-  </si>
-  <si>
     <t>《櫻木花道大危機!!》Postcard　／SLAM DUNK　Goods　BY：波小姐(LADY PO)（我們果真是天才）</t>
   </si>
   <si>
@@ -160,45 +142,30 @@
     <t>$40</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/36/361009bd6cfcc1fd7d71196ef24f9150.jpg</t>
-  </si>
-  <si>
     <t>《少根筋的他與雙胞胎兔子》　／Original　Comic　BY：地獄道長</t>
   </si>
   <si>
     <t>https://fanhouse.waca.ec/en/product/detail/1772263</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/3e/3e88ed3d2ea7f20cc79daa74bf6d4a33.jpg</t>
-  </si>
-  <si>
     <t>《耀眼的他與陰沉的兔子》　／Original　Comic　BY：地獄道長</t>
   </si>
   <si>
     <t>https://fanhouse.waca.ec/en/product/detail/1772257</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/ae/ae2df0fbb84022cd04fe33fa4c82c521.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】Lukejamie Acrylic Charm　／Street Fighter　Luke Sullivan/Jamie Siu　Goods　BY：米乓</t>
   </si>
   <si>
     <t>https://fanhouse.waca.ec/en/product/detail/1771841</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/49/49ea6f0178f1b018ef979b9ff646810e.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】LUKE &amp; JAMIE Sticker　／Street Fighter　Luke Sullivan/Jamie Siu　Goods　BY：米乓</t>
   </si>
   <si>
     <t>https://fanhouse.waca.ec/en/product/detail/1771821</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/8e/8eb032bcf0fb3bdc4584dba403e7647f.jpg</t>
-  </si>
-  <si>
     <t>【PRE-SALE】LUKE &amp; JAMIE Acrylic Stands Set　／Street Fighter　Luke Sullivan/Jamie Siu　Goods　BY：米乓</t>
   </si>
   <si>
@@ -208,9 +175,6 @@
     <t>$200</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/10/1013371f90df83bb8569bb69428f5fb8.jpg</t>
-  </si>
-  <si>
     <t>《HEY CHAT!》Posters &amp; Cards Set　／Nijisanji-EN／VTuber　Goods　BY：跋倒（庠隱）</t>
   </si>
   <si>
@@ -220,9 +184,6 @@
     <t>$120 ~ 280</t>
   </si>
   <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/3c/3c8f16163776b4d0aaa2e9dbb9f0b0d4.jpg</t>
-  </si>
-  <si>
     <t>《HEY CHAT!》　／Nijisanji-EN／VTuber　Illustration Book　BY：跋倒（庠隱）</t>
   </si>
   <si>
@@ -230,40 +191,13 @@
   </si>
   <si>
     <t>$60 ~ 980</t>
-  </si>
-  <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/27/27a4b8ba6502f779b55d95bfc639be59.jpg</t>
-  </si>
-  <si>
-    <t>《Minista》Acrylic Blocks　／Nijisanji-EN／VTuber　Goods　BY：跋倒（庠隱）</t>
-  </si>
-  <si>
-    <t>https://fanhouse.waca.ec/en/product/detail/1767643</t>
-  </si>
-  <si>
-    <t>$180 ~ 900</t>
-  </si>
-  <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/4d/4df969ffa03ee32eda382e51ea1eb192.jpg</t>
-  </si>
-  <si>
-    <t>《Minista》Puffy Stickers　／Nijisanji-EN／VTuber　Goods　BY：跋倒（庠隱）</t>
-  </si>
-  <si>
-    <t>https://fanhouse.waca.ec/en/product/detail/1767641</t>
-  </si>
-  <si>
-    <t>$140</t>
-  </si>
-  <si>
-    <t>https://wacaimg1.waca.ec/uploads/shops/3388/products/87/872948d4468e99c4b427af25549589c1.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,13 +212,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -304,20 +231,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -329,20 +253,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>4062413</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="6fb83165c565e5c48269915702968b58.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="87b1029f9e0b44013bdce04d241cf24c.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -355,32 +279,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="190500"/>
-          <a:ext cx="2857500" cy="4062413"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="190500"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>4086225</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="f9683146ece7dd269bfea62f9314e914.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr="ac9973a51b09ef6611d08fef1c276f4a.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -393,32 +317,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="5600700"/>
-          <a:ext cx="2857500" cy="4086225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="4419600"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>2738438</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3" descr="d5d4e6d9ad80ccc7210048e9230474f2.jpg"/>
+      <xdr:rowOff>5687377</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="6fb83165c565e5c48269915702968b58.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -431,32 +355,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="11049000"/>
-          <a:ext cx="2857500" cy="2738438"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="8648700"/>
+          <a:ext cx="4000500" cy="5687377"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2643188</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4" descr="2b238394cd780ff1c27b43d221210b94.jpg"/>
+      <xdr:rowOff>5720715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="f9683146ece7dd269bfea62f9314e914.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -469,32 +393,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="14697075"/>
-          <a:ext cx="2857500" cy="2643188"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="14658975"/>
+          <a:ext cx="4000500" cy="5720715"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5" descr="8e307e5a772e9fe6d878a8998376fd6d.jpg"/>
+      <xdr:rowOff>3833813</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="d5d4e6d9ad80ccc7210048e9230474f2.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -507,32 +431,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="18221325"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="20707350"/>
+          <a:ext cx="4000500" cy="3833813"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2038350</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6" descr="c00bc0fc4cd46c5fa96280976b4724aa.jpg"/>
+      <xdr:rowOff>3700463</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="2b238394cd780ff1c27b43d221210b94.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -545,32 +469,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="22031325"/>
-          <a:ext cx="2857500" cy="2038350"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="24755475"/>
+          <a:ext cx="4000500" cy="3700463"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>4043363</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7" descr="fae8ecd0ab5eaf3fb0663f52c4ddc581.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="8e307e5a772e9fe6d878a8998376fd6d.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -583,32 +507,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="24745950"/>
-          <a:ext cx="2857500" cy="4043363"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="28670250"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>2967038</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8" descr="def32dcb6932cb2a8f0ee0dae1a91180.jpg"/>
+      <xdr:rowOff>2853690</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="c00bc0fc4cd46c5fa96280976b4724aa.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -621,32 +545,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="30137100"/>
-          <a:ext cx="2857500" cy="2967038"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="32899350"/>
+          <a:ext cx="4000500" cy="2853690"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>3214688</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9" descr="9aee0539060d12ac654e04a62f64e04f.jpg"/>
+      <xdr:rowOff>5660708</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="fae8ecd0ab5eaf3fb0663f52c4ddc581.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -659,32 +583,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="34089975"/>
-          <a:ext cx="2857500" cy="3214688"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="35918775"/>
+          <a:ext cx="4000500" cy="5660708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10" descr="4afdbaffd8a2934af06a3c211b94fca7.jpg"/>
+      <xdr:rowOff>4153852</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10" descr="def32dcb6932cb2a8f0ee0dae1a91180.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -697,32 +621,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="38376225"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="41900475"/>
+          <a:ext cx="4000500" cy="4153852"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Picture 11" descr="361009bd6cfcc1fd7d71196ef24f9150.jpg"/>
+      <xdr:rowOff>4500562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="9aee0539060d12ac654e04a62f64e04f.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -735,32 +659,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="42186225"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="46291500"/>
+          <a:ext cx="4000500" cy="4500562"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>4067175</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="13" name="Picture 12" descr="3e88ed3d2ea7f20cc79daa74bf6d4a33.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12" descr="4afdbaffd8a2934af06a3c211b94fca7.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -773,32 +697,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="45996225"/>
-          <a:ext cx="2857500" cy="4067175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="51054000"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>4062413</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Picture 13" descr="ae2df0fbb84022cd04fe33fa4c82c521.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13" descr="361009bd6cfcc1fd7d71196ef24f9150.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -811,32 +735,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="51415950"/>
-          <a:ext cx="2857500" cy="4062413"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="55283100"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14" descr="49ea6f0178f1b018ef979b9ff646810e.jpg"/>
+      <xdr:rowOff>5694045</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14" descr="3e88ed3d2ea7f20cc79daa74bf6d4a33.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -849,32 +773,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="56826150"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="59512200"/>
+          <a:ext cx="4000500" cy="5694045"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Picture 15" descr="8eb032bcf0fb3bdc4584dba403e7647f.jpg"/>
+      <xdr:rowOff>5687377</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15" descr="ae2df0fbb84022cd04fe33fa4c82c521.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -887,32 +811,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="60636150"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="65532000"/>
+          <a:ext cx="4000500" cy="5687377"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>2828925</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16" descr="1013371f90df83bb8569bb69428f5fb8.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16" descr="49ea6f0178f1b018ef979b9ff646810e.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -925,32 +849,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="64446150"/>
-          <a:ext cx="2857500" cy="2828925"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="71542275"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17" descr="3c8f16163776b4d0aaa2e9dbb9f0b0d4.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17" descr="8eb032bcf0fb3bdc4584dba403e7647f.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -963,32 +887,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="68218050"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="75771375"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="19" name="Picture 18" descr="27a4b8ba6502f779b55d95bfc639be59.jpg"/>
+      <xdr:rowOff>3960495</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18" descr="1013371f90df83bb8569bb69428f5fb8.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1001,32 +925,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="72028050"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="80000475"/>
+          <a:ext cx="4000500" cy="3960495"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Picture 19" descr="4df969ffa03ee32eda382e51ea1eb192.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="3c8f16163776b4d0aaa2e9dbb9f0b0d4.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1039,32 +963,32 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="75838050"/>
-          <a:ext cx="2857500" cy="2857500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
+          <a:off x="6419850" y="84191475"/>
+          <a:ext cx="4000500" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2857500</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4000500</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>2857500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="Picture 20" descr="872948d4468e99c4b427af25549589c1.jpg"/>
+      <xdr:rowOff>4000500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20" descr="27a4b8ba6502f779b55d95bfc639be59.jpg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1077,8 +1001,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17678400" y="79648050"/>
-          <a:ext cx="2857500" cy="2857500"/>
+          <a:off x="6419850" y="88420575"/>
+          <a:ext cx="4000500" cy="4000500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1375,21 +1299,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="111.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="91.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="300.7109375" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="75.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1405,348 +1327,285 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="426.5" customHeight="1">
+    </row>
+    <row r="2" spans="1:5" ht="333.333" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="429" customHeight="1">
+    </row>
+    <row r="3" spans="1:5" ht="333.333" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="287.5" customHeight="1">
+    </row>
+    <row r="4" spans="1:5" ht="473.889" customHeight="1">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="277.5" customHeight="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="476.667" customHeight="1">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="300" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="319.444" customHeight="1">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="214" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="308.333" customHeight="1">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>26</v>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="424.5" customHeight="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="333.333" customHeight="1">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="311.5" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="237.778" customHeight="1">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>34</v>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="337.5" customHeight="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="471.667" customHeight="1">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>37</v>
+      <c r="B10" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="300" customHeight="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="346.111" customHeight="1">
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>41</v>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="300" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="375" customHeight="1">
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>45</v>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="427" customHeight="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="333.333" customHeight="1">
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>49</v>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="426.5" customHeight="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="333.333" customHeight="1">
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>52</v>
+      <c r="B14" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="300" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="474.444" customHeight="1">
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>55</v>
+      <c r="B15" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="300" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="473.889" customHeight="1">
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>58</v>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="297" customHeight="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="333.333" customHeight="1">
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>61</v>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="300" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="333.333" customHeight="1">
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>65</v>
+      <c r="B18" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="300" customHeight="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="330" customHeight="1">
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>69</v>
+      <c r="B19" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="300" customHeight="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="333.333" customHeight="1">
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>73</v>
+      <c r="B20" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="300" customHeight="1">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="333.333" customHeight="1">
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
-        <v>77</v>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>